<commit_message>
1. Added Expand Collapse feature 2. warning message when change in dataset and if annotation were saved 3. Added Annotation Toggle
</commit_message>
<xml_diff>
--- a/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\KPIColumn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitlab\documents\Published\KPIColumn\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7909B66-CEB9-4193-B3C4-2BE8D7E23072}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
   </bookViews>
@@ -340,9 +341,6 @@
 3. Legends will be removed the visual</t>
   </si>
   <si>
-    <t>Update data label's color, text size, display units and decimal value</t>
-  </si>
-  <si>
     <t>1. Data label will be visible in the visual above each bar
 2. Data labels color will be set to 'black'
 3. Data labels text size will be resized to '14' pt.
@@ -375,9 +373,6 @@
     <t>Adding ToolTip</t>
   </si>
   <si>
-    <t>Add a tooltip for additional information</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adding one or more column to the tooltip bag.  </t>
   </si>
   <si>
@@ -471,6 +466,12 @@
 2. If stroke value is '-2' then it will automatically change to '1'
 3. If stroke value is '7' then it will automatically change to '5'
 4. The target line should disappear</t>
+  </si>
+  <si>
+    <t>Add a tooltip for additional information on bars and individual target points(displayed only individual target).</t>
+  </si>
+  <si>
+    <t>Update data label's color, text size, display units and decimal value(Max text size is 20)</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C560CE-405B-4CA8-AB3A-A0EEBCD256B2}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1123,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1167,7 +1168,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1201,7 +1202,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1229,13 +1230,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1260,16 +1261,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1277,16 +1278,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1294,16 +1295,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1311,16 +1312,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1328,16 +1329,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1345,16 +1346,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1597,7 +1598,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1676,13 +1677,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1690,10 +1691,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1701,10 +1702,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1712,10 +1713,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2"/>
     </row>

</xml_diff>